<commit_message>
add kiran and modified
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Git_Tutorial\1\asdf\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E03E12-C743-438E-8F51-C345CE8FFF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +25,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +34,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +68,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +351,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>